<commit_message>
[LPF-626]: Create CCMS Invoice Analysis report
Signed-off-by: robert.buczek <robert.buczek@digital.justice.gov.uk>
</commit_message>
<xml_diff>
--- a/src/main/resources/CCMS_invoice analysis_template_v1_1.xlsx
+++ b/src/main/resources/CCMS_invoice analysis_template_v1_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason.smallman/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert.buczek/Projects/payforlegalaid/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65109B52-4BCD-8D46-B180-A066DBFE7EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E339FD8-B62A-2847-BF18-8EAB650F32F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" tabRatio="842" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="13" r:id="rId1"/>
@@ -27,8 +27,8 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
-    <pivotCache cacheId="1" r:id="rId9"/>
+    <pivotCache cacheId="28" r:id="rId8"/>
+    <pivotCache cacheId="29" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1047,7 +1047,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000001000000}" name="ByProviderPivot" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption=" " updatedVersion="8" minRefreshableVersion="3" showCalcMbrs="0" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Office code">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000001000000}" name="ByProviderPivot" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption=" " updatedVersion="8" minRefreshableVersion="3" showCalcMbrs="0" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Office code">
   <location ref="A52:C55" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" showAll="0">
@@ -1105,7 +1105,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C970B8B3-04A9-4FBE-8F9D-09BCF93CAB04}" name="ByDayPivot" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showCalcMbrs="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Day of week" colHeaderCaption=" ">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C970B8B3-04A9-4FBE-8F9D-09BCF93CAB04}" name="ByDayPivot" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showCalcMbrs="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Day of week" colHeaderCaption=" ">
   <location ref="A18:C21" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -1506,8 +1506,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:O644"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1610,13 +1610,13 @@
       <c r="A12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="13" t="e">
-        <f>COUNTIF('CCMS AP Debtors'!#REF!,"&lt;0")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C12" s="2" t="e">
-        <f>SUM('CCMS AP Debtors'!#REF!)</f>
-        <v>#REF!</v>
+      <c r="B12" s="13">
+        <f>COUNTIF('CCMS AP Debtors'!E:E,"&lt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <f>SUM('CCMS AP Debtors'!E:E)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -3864,7 +3864,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -3907,6 +3907,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="69644ca7-2514-4c9e-ac84-a1727a156c0c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ca99a096-e482-44e0-b523-c2fa9d17e452" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050B3361E0499424DBCAEEF99972D696F" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8f19487a894dd6a08332a2d0e568621e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69644ca7-2514-4c9e-ac84-a1727a156c0c" xmlns:ns3="ca99a096-e482-44e0-b523-c2fa9d17e452" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b486a0c41fdd39eab1282f012448fcb0" ns2:_="" ns3:_="">
     <xsd:import namespace="69644ca7-2514-4c9e-ac84-a1727a156c0c"/>
@@ -4137,17 +4148,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="69644ca7-2514-4c9e-ac84-a1727a156c0c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ca99a096-e482-44e0-b523-c2fa9d17e452" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5210BC3-5B5D-4169-8DEE-68F2E793F77D}">
   <ds:schemaRefs>
@@ -4157,6 +4157,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B7F9D9C-8E7C-4BB2-AF18-32B53426902F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="69644ca7-2514-4c9e-ac84-a1727a156c0c"/>
+    <ds:schemaRef ds:uri="ca99a096-e482-44e0-b523-c2fa9d17e452"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C9EA5EA-03BA-4751-9150-B01397226F2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4173,15 +4184,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B7F9D9C-8E7C-4BB2-AF18-32B53426902F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="69644ca7-2514-4c9e-ac84-a1727a156c0c"/>
-    <ds:schemaRef ds:uri="ca99a096-e482-44e0-b523-c2fa9d17e452"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>